<commit_message>
balikan Topup + tambah TC
</commit_message>
<xml_diff>
--- a/Simulasi/Simulasi Hitung Top Up Using Coupon.xlsx
+++ b/Simulasi/Simulasi Hitung Top Up Using Coupon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KIP'\Katalon Test\EENDIGOProject\Simulasi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B45D0B-F9F7-416A-BCE3-AA5A41940910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C048BBD6-1F01-4BE1-BFB1-EC8277905B33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TopUp Disc Percent" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="26">
   <si>
     <t>Service</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Total Cashback</t>
   </si>
   <si>
-    <t>OCR BPKB</t>
-  </si>
-  <si>
     <t>Jumlah</t>
   </si>
   <si>
@@ -51,12 +48,6 @@
     <t>Price</t>
   </si>
   <si>
-    <t>OCR NPWP</t>
-  </si>
-  <si>
-    <t>&lt;dst&gt;</t>
-  </si>
-  <si>
     <t>Sub Total</t>
   </si>
   <si>
@@ -112,6 +103,9 @@
   </si>
   <si>
     <t>Grand Total Cashback</t>
+  </si>
+  <si>
+    <t>3000</t>
   </si>
 </sst>
 </file>
@@ -463,7 +457,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -482,46 +476,46 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D2" t="str">
         <f>IFERROR(B2*C2,"")</f>
         <v/>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F2" t="str">
         <f xml:space="preserve"> IFERROR(ROUNDDOWN(D2*E2/100,0),"")</f>
@@ -542,20 +536,20 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D15" si="0">IFERROR(B3*C3,"")</f>
         <v/>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F15" si="1" xml:space="preserve"> IFERROR(ROUNDDOWN(D3*E3/100,0),"")</f>
@@ -576,14 +570,14 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="1"/>
@@ -608,7 +602,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="1"/>
@@ -633,7 +627,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="1"/>
@@ -658,7 +652,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="1"/>
@@ -683,7 +677,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="1"/>
@@ -708,7 +702,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="1"/>
@@ -733,7 +727,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="1"/>
@@ -758,7 +752,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="1"/>
@@ -783,7 +777,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="1"/>
@@ -808,7 +802,7 @@
         <v>0</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="1"/>
@@ -833,7 +827,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="1"/>
@@ -858,7 +852,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="1"/>
@@ -879,7 +873,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B17">
         <f>SUM(D$2:D$15)</f>
@@ -888,7 +882,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B18">
         <f>SUM(F$2:F$15)</f>
@@ -897,7 +891,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B19">
         <f>SUM(H$2:H$15)</f>
@@ -906,7 +900,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B20">
         <f>SUM(I$2:I$15)</f>
@@ -916,7 +910,7 @@
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -932,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -947,48 +941,48 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1">
-        <v>501</v>
-      </c>
-      <c r="C2" s="1">
-        <v>100</v>
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>500</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
       </c>
       <c r="D2">
         <f>IFERROR(B2*C2,"")</f>
-        <v>50100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>501</v>
+      </c>
+      <c r="C3">
         <v>7</v>
-      </c>
-      <c r="B3" s="1">
-        <v>720</v>
-      </c>
-      <c r="C3" s="1">
-        <v>10</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D15" si="0">IFERROR(B3*C3,"")</f>
-        <v>7200</v>
+        <v>3507</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
@@ -1063,52 +1057,52 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="1">
-        <v>3000</v>
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <f>SUM($D$2:$D$15)</f>
+        <v>9507</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B18">
-        <f>IFERROR(SUM(D$2:D$15),"")</f>
-        <v>57300</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B19">
-        <f>B18-B17</f>
-        <v>54300</v>
+        <f>IFERROR(ROUNDDOWN(B21*11%,0),"")</f>
+        <v>495</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B20">
-        <f>IFERROR(ROUNDDOWN(B19*11%,0),"")</f>
-        <v>5973</v>
+        <f>IFERROR(ROUNDDOWN(B19+B21,0),"")</f>
+        <v>5002</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B21">
-        <f>IFERROR(ROUNDDOWN(B19+B20,0),"")</f>
-        <v>60273</v>
+        <f>IFERROR(ROUNDDOWN(B17-B18,0),"")</f>
+        <v>4507</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1120,8 +1114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1140,28 +1134,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -1214,7 +1208,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F4" t="str">
         <f>IFERROR(ROUNDDOWN(D4*E4/100,0), "")</f>
@@ -1239,7 +1233,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" ref="F5:F15" si="4">IFERROR(ROUNDDOWN(D5*E5/100,0), "")</f>
@@ -1264,7 +1258,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="4"/>
@@ -1289,7 +1283,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="4"/>
@@ -1314,7 +1308,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="4"/>
@@ -1339,7 +1333,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="4"/>
@@ -1364,7 +1358,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="4"/>
@@ -1389,7 +1383,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="4"/>
@@ -1414,7 +1408,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="4"/>
@@ -1439,7 +1433,7 @@
         <v>0</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="4"/>
@@ -1464,7 +1458,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="4"/>
@@ -1507,7 +1501,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B17">
         <f>SUM(D$2:D$14)</f>
@@ -1516,7 +1510,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B18">
         <f>SUM(F$2:F$15)</f>
@@ -1525,16 +1519,16 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B19">
-        <f>B17*11%</f>
+        <f>IFERROR(B18-B17,"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B20">
         <f>B17+B19</f>
@@ -1544,7 +1538,7 @@
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1557,7 +1551,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1575,104 +1569,104 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1">
-        <v>501</v>
-      </c>
-      <c r="C2" s="1">
-        <v>100</v>
-      </c>
-      <c r="D2">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="str">
         <f>IFERROR(B2*C2,"")</f>
-        <v>50100</v>
-      </c>
-      <c r="E2" s="5">
+        <v/>
+      </c>
+      <c r="E2" s="5" t="str">
         <f>IFERROR(D2/SUM(D$2:D$15),"")</f>
-        <v>0.58188153310104529</v>
-      </c>
-      <c r="F2" s="4">
-        <f>IFERROR($B$17*E2,"")</f>
-        <v>2909.4076655052263</v>
-      </c>
-      <c r="G2" s="6">
+        <v/>
+      </c>
+      <c r="F2" s="4" t="str">
+        <f t="shared" ref="F2:F15" si="0">IFERROR($B$18*E2,"")</f>
+        <v/>
+      </c>
+      <c r="G2" s="6" t="str">
         <f>IFERROR(ROUNDDOWN(F2/B2,0),"")</f>
-        <v>5</v>
-      </c>
-      <c r="H2" s="6">
+        <v/>
+      </c>
+      <c r="H2" s="6" t="str">
         <f>IFERROR(C2+G2,"")</f>
-        <v>105</v>
+        <v/>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1">
-        <v>720</v>
-      </c>
-      <c r="C3" s="1">
-        <v>50</v>
-      </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D15" si="0">IFERROR(B3*C3,"")</f>
-        <v>36000</v>
-      </c>
-      <c r="E3" s="5">
-        <f t="shared" ref="E3:E15" si="1">IFERROR(D3/SUM(D$2:D$15),"")</f>
-        <v>0.41811846689895471</v>
-      </c>
-      <c r="F3" s="4">
-        <f t="shared" ref="F3:F15" si="2">IFERROR($B$17*E3,"")</f>
-        <v>2090.5923344947737</v>
-      </c>
-      <c r="G3" s="6">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D15" si="1">IFERROR(B3*C3,"")</f>
+        <v/>
+      </c>
+      <c r="E3" s="5" t="str">
+        <f t="shared" ref="E3:E15" si="2">IFERROR(D3/SUM(D$2:D$15),"")</f>
+        <v/>
+      </c>
+      <c r="F3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G3" s="6" t="str">
         <f t="shared" ref="G3:G15" si="3">IFERROR(ROUNDDOWN(F3/B3,0),"")</f>
-        <v>2</v>
-      </c>
-      <c r="H3" s="6">
+        <v/>
+      </c>
+      <c r="H3" s="6" t="str">
         <f t="shared" ref="H3:H15" si="4">IFERROR(C3+G3,"")</f>
-        <v>52</v>
+        <v/>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E4" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F4" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E4" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="F4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="G4" s="6" t="str">
         <f t="shared" si="3"/>
@@ -1685,16 +1679,16 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E5" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F5" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E5" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="F5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="G5" s="6" t="str">
         <f t="shared" si="3"/>
@@ -1707,16 +1701,16 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E6" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F6" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E6" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="F6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="G6" s="6" t="str">
         <f t="shared" si="3"/>
@@ -1729,16 +1723,16 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E7" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F7" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E7" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="F7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="G7" s="6" t="str">
         <f t="shared" si="3"/>
@@ -1751,16 +1745,16 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E8" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F8" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E8" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="F8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="G8" s="6" t="str">
         <f t="shared" si="3"/>
@@ -1773,16 +1767,16 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E9" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E9" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="F9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="G9" s="6" t="str">
         <f t="shared" si="3"/>
@@ -1795,16 +1789,16 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E10" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F10" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E10" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="F10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="G10" s="6" t="str">
         <f t="shared" si="3"/>
@@ -1817,16 +1811,16 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E11" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E11" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="F11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="G11" s="6" t="str">
         <f t="shared" si="3"/>
@@ -1839,16 +1833,16 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E12" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E12" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="F12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="G12" s="6" t="str">
         <f t="shared" si="3"/>
@@ -1861,16 +1855,16 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E13" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F13" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E13" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="F13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="G13" s="6" t="str">
         <f t="shared" si="3"/>
@@ -1883,16 +1877,16 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E14" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F14" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="F14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="G14" s="6" t="str">
         <f t="shared" si="3"/>
@@ -1905,16 +1899,16 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E15" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E15" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="F15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="G15" s="6" t="str">
         <f t="shared" si="3"/>
@@ -1927,43 +1921,43 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="1">
-        <v>5000</v>
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <f>SUM(D$2:D$15)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18">
-        <f>SUM(D$2:D$15)</f>
-        <v>86100</v>
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B19">
-        <f>B18*11%</f>
-        <v>9471</v>
+        <f>IFERROR(ROUNDDOWN(B17*11%,0),"")</f>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B20">
-        <f>B18+B19</f>
-        <v>95571</v>
+        <f>IFERROR(B17+B19,"")</f>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
udpate apiaas 6 feb
</commit_message>
<xml_diff>
--- a/Simulasi/Simulasi Hitung Top Up Using Coupon.xlsx
+++ b/Simulasi/Simulasi Hitung Top Up Using Coupon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KIP'\Katalon Test\EENDIGOProject\Simulasi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{A9265993-EAF5-4361-9046-10035A6B241C}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{6A8E376A-C859-4CD8-9F58-A548CF0FC4AB}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
     <workbookView windowHeight="10420" windowWidth="19420" xWindow="-110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-110"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="32">
   <si>
     <t>Service</t>
   </si>
@@ -1622,13 +1622,13 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <f>IFERROR(B2*C2,"")</f>
@@ -1653,13 +1653,13 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="D3">
         <f ref="D3:D15" si="1" t="shared">IFERROR(B3*C3,"")</f>
@@ -1963,7 +1963,7 @@
         <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:2">

</xml_diff>